<commit_message>
plots of HFD enriched taxa
</commit_message>
<xml_diff>
--- a/metadata/hfd_02wk_raw_metadata/hfd_02wk_metadata_raw.xlsx
+++ b/metadata/hfd_02wk_raw_metadata/hfd_02wk_metadata_raw.xlsx
@@ -3,24 +3,35 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69B0FF1B-196D-A741-9B5C-B2FEC2016875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A43A4F3-A5F0-3B4B-BF31-4E938AC2D227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="500" windowWidth="16640" windowHeight="21500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="16640" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="229">
   <si>
     <t>Sample Name</t>
   </si>
@@ -621,6 +632,96 @@
   </si>
   <si>
     <t>Luminal</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>jejunum</t>
+  </si>
+  <si>
+    <t>ileum</t>
+  </si>
+  <si>
+    <t>cecum</t>
+  </si>
+  <si>
+    <t>colon</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>LFD</t>
+  </si>
+  <si>
+    <t>HFD</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>656,</t>
+  </si>
+  <si>
+    <t>con</t>
+  </si>
+  <si>
+    <t>657,</t>
+  </si>
+  <si>
+    <t>658,</t>
+  </si>
+  <si>
+    <t>659,</t>
+  </si>
+  <si>
+    <t>660,</t>
+  </si>
+  <si>
+    <t>651,</t>
+  </si>
+  <si>
+    <t>652,</t>
+  </si>
+  <si>
+    <t>653,</t>
+  </si>
+  <si>
+    <t>654,</t>
+  </si>
+  <si>
+    <t>655,</t>
+  </si>
+  <si>
+    <t>A (651)</t>
+  </si>
+  <si>
+    <t>B (652)</t>
+  </si>
+  <si>
+    <t>C (653)</t>
+  </si>
+  <si>
+    <t>D (654)</t>
+  </si>
+  <si>
+    <t>E (655)</t>
+  </si>
+  <si>
+    <t>C5 (660)</t>
+  </si>
+  <si>
+    <t>C1 (656)</t>
+  </si>
+  <si>
+    <t>C2 (657)</t>
+  </si>
+  <si>
+    <t>C3 (658)</t>
+  </si>
+  <si>
+    <t>C4 (659)</t>
   </si>
 </sst>
 </file>
@@ -723,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -773,6 +874,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M91"/>
+  <dimension ref="B1:AO91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="AO37" sqref="AO1:AO1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1065,8 +1167,7 @@
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
     <col min="4" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="6" max="7" width="18.1640625" customWidth="1"/>
     <col min="8" max="9" width="17.1640625" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" customWidth="1"/>
   </cols>
@@ -1076,6 +1177,11 @@
         <v>183</v>
       </c>
     </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>32</v>
@@ -1109,6 +1215,12 @@
       <c r="F4" s="1">
         <v>4.9400000000000004</v>
       </c>
+      <c r="G4" t="s">
+        <v>219</v>
+      </c>
+      <c r="H4" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
@@ -1126,6 +1238,12 @@
       <c r="F5" s="1">
         <v>8.1</v>
       </c>
+      <c r="G5" t="s">
+        <v>219</v>
+      </c>
+      <c r="H5" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1143,6 +1261,12 @@
       <c r="F6" s="10">
         <v>70.34</v>
       </c>
+      <c r="G6" t="s">
+        <v>219</v>
+      </c>
+      <c r="H6" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
@@ -1160,6 +1284,12 @@
       <c r="F7" s="10">
         <v>37.25</v>
       </c>
+      <c r="G7" t="s">
+        <v>219</v>
+      </c>
+      <c r="H7" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="8" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
@@ -1177,6 +1307,12 @@
       <c r="F8" s="10">
         <v>3.49</v>
       </c>
+      <c r="G8" t="s">
+        <v>220</v>
+      </c>
+      <c r="H8" t="s">
+        <v>200</v>
+      </c>
       <c r="L8" s="12" t="s">
         <v>99</v>
       </c>
@@ -1200,6 +1336,12 @@
       <c r="F9" s="10">
         <v>6.57</v>
       </c>
+      <c r="G9" t="s">
+        <v>220</v>
+      </c>
+      <c r="H9" t="s">
+        <v>201</v>
+      </c>
       <c r="L9" s="12"/>
       <c r="M9" s="15"/>
     </row>
@@ -1219,6 +1361,12 @@
       <c r="F10" s="10">
         <v>56.2</v>
       </c>
+      <c r="G10" t="s">
+        <v>220</v>
+      </c>
+      <c r="H10" t="s">
+        <v>202</v>
+      </c>
       <c r="L10" s="12"/>
       <c r="M10" s="15"/>
     </row>
@@ -1238,6 +1386,12 @@
       <c r="F11" s="10">
         <v>27.46</v>
       </c>
+      <c r="G11" t="s">
+        <v>220</v>
+      </c>
+      <c r="H11" t="s">
+        <v>203</v>
+      </c>
       <c r="L11" s="12"/>
       <c r="M11" s="15"/>
     </row>
@@ -1257,6 +1411,12 @@
       <c r="F12" s="10">
         <v>3.6</v>
       </c>
+      <c r="G12" t="s">
+        <v>221</v>
+      </c>
+      <c r="H12" t="s">
+        <v>200</v>
+      </c>
       <c r="L12" s="12"/>
       <c r="M12" s="15"/>
     </row>
@@ -1276,6 +1436,12 @@
       <c r="F13" s="10">
         <v>6.03</v>
       </c>
+      <c r="G13" t="s">
+        <v>221</v>
+      </c>
+      <c r="H13" t="s">
+        <v>201</v>
+      </c>
       <c r="L13" s="12"/>
       <c r="M13" s="15"/>
     </row>
@@ -1295,6 +1461,12 @@
       <c r="F14" s="10">
         <v>116</v>
       </c>
+      <c r="G14" t="s">
+        <v>221</v>
+      </c>
+      <c r="H14" t="s">
+        <v>202</v>
+      </c>
       <c r="L14" s="14" t="s">
         <v>33</v>
       </c>
@@ -1316,6 +1488,12 @@
       <c r="F15" s="10">
         <v>12.69</v>
       </c>
+      <c r="G15" t="s">
+        <v>221</v>
+      </c>
+      <c r="H15" t="s">
+        <v>203</v>
+      </c>
       <c r="L15" s="14"/>
       <c r="M15" s="15"/>
     </row>
@@ -1335,6 +1513,12 @@
       <c r="F16" s="10">
         <v>4.1399999999999997</v>
       </c>
+      <c r="G16" t="s">
+        <v>222</v>
+      </c>
+      <c r="H16" t="s">
+        <v>200</v>
+      </c>
       <c r="L16" s="14"/>
       <c r="M16" s="15"/>
     </row>
@@ -1354,6 +1538,12 @@
       <c r="F17" s="10">
         <v>6.3</v>
       </c>
+      <c r="G17" t="s">
+        <v>222</v>
+      </c>
+      <c r="H17" t="s">
+        <v>201</v>
+      </c>
       <c r="L17" s="14"/>
       <c r="M17" s="15"/>
     </row>
@@ -1373,6 +1563,12 @@
       <c r="F18" s="10">
         <v>47.49</v>
       </c>
+      <c r="G18" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" t="s">
+        <v>202</v>
+      </c>
       <c r="L18" s="14"/>
       <c r="M18" s="15"/>
     </row>
@@ -1392,6 +1588,12 @@
       <c r="F19" s="10">
         <v>38.090000000000003</v>
       </c>
+      <c r="G19" t="s">
+        <v>222</v>
+      </c>
+      <c r="H19" t="s">
+        <v>203</v>
+      </c>
       <c r="L19" s="14"/>
       <c r="M19" s="15"/>
     </row>
@@ -1411,6 +1613,12 @@
       <c r="F20" s="10">
         <v>7.65</v>
       </c>
+      <c r="G20" t="s">
+        <v>223</v>
+      </c>
+      <c r="H20" t="s">
+        <v>200</v>
+      </c>
       <c r="L20" s="13" t="s">
         <v>100</v>
       </c>
@@ -1432,6 +1640,12 @@
       <c r="F21" s="10">
         <v>4.57</v>
       </c>
+      <c r="G21" t="s">
+        <v>223</v>
+      </c>
+      <c r="H21" t="s">
+        <v>201</v>
+      </c>
       <c r="L21" s="13"/>
       <c r="M21" s="15"/>
     </row>
@@ -1451,6 +1665,12 @@
       <c r="F22" s="10">
         <v>79.11</v>
       </c>
+      <c r="G22" t="s">
+        <v>223</v>
+      </c>
+      <c r="H22" t="s">
+        <v>202</v>
+      </c>
       <c r="L22" s="13"/>
       <c r="M22" s="15"/>
     </row>
@@ -1470,6 +1690,12 @@
       <c r="F23" s="10">
         <v>18.7</v>
       </c>
+      <c r="G23" t="s">
+        <v>223</v>
+      </c>
+      <c r="H23" t="s">
+        <v>203</v>
+      </c>
       <c r="L23" s="13"/>
       <c r="M23" s="15"/>
     </row>
@@ -1489,6 +1715,12 @@
       <c r="F24" s="10">
         <v>3.52</v>
       </c>
+      <c r="G24" t="s">
+        <v>225</v>
+      </c>
+      <c r="H24" t="s">
+        <v>200</v>
+      </c>
       <c r="L24" s="13"/>
       <c r="M24" s="15"/>
     </row>
@@ -1508,6 +1740,12 @@
       <c r="F25" s="10">
         <v>20.5</v>
       </c>
+      <c r="G25" t="s">
+        <v>225</v>
+      </c>
+      <c r="H25" t="s">
+        <v>201</v>
+      </c>
       <c r="L25" s="13"/>
       <c r="M25" s="15"/>
     </row>
@@ -1527,6 +1765,12 @@
       <c r="F26" s="10">
         <v>726.9</v>
       </c>
+      <c r="G26" t="s">
+        <v>225</v>
+      </c>
+      <c r="H26" t="s">
+        <v>202</v>
+      </c>
       <c r="L26" s="6"/>
       <c r="M26" s="16" t="s">
         <v>184</v>
@@ -1548,6 +1792,12 @@
       <c r="F27" s="10">
         <v>66.67</v>
       </c>
+      <c r="G27" t="s">
+        <v>225</v>
+      </c>
+      <c r="H27" t="s">
+        <v>203</v>
+      </c>
       <c r="L27" s="7"/>
       <c r="M27" s="16"/>
     </row>
@@ -1567,6 +1817,12 @@
       <c r="F28" s="10">
         <v>7.59</v>
       </c>
+      <c r="G28" t="s">
+        <v>226</v>
+      </c>
+      <c r="H28" t="s">
+        <v>200</v>
+      </c>
       <c r="L28" s="8"/>
       <c r="M28" s="16"/>
     </row>
@@ -1586,6 +1842,12 @@
       <c r="F29" s="10">
         <v>6.47</v>
       </c>
+      <c r="G29" t="s">
+        <v>226</v>
+      </c>
+      <c r="H29" t="s">
+        <v>201</v>
+      </c>
       <c r="L29" s="9"/>
       <c r="M29" s="16"/>
     </row>
@@ -1605,6 +1867,12 @@
       <c r="F30" s="10">
         <v>69.040000000000006</v>
       </c>
+      <c r="G30" t="s">
+        <v>226</v>
+      </c>
+      <c r="H30" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
@@ -1622,6 +1890,12 @@
       <c r="F31" s="10">
         <v>43.9</v>
       </c>
+      <c r="G31" t="s">
+        <v>226</v>
+      </c>
+      <c r="H31" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
@@ -1639,8 +1913,14 @@
       <c r="F32" s="10">
         <v>9.25</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>227</v>
+      </c>
+      <c r="H32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>76</v>
       </c>
@@ -1656,8 +1936,14 @@
       <c r="F33" s="10">
         <v>10.4</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>227</v>
+      </c>
+      <c r="H33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>77</v>
       </c>
@@ -1673,8 +1959,14 @@
       <c r="F34" s="10">
         <v>76.47</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>227</v>
+      </c>
+      <c r="H34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>78</v>
       </c>
@@ -1690,8 +1982,14 @@
       <c r="F35" s="10">
         <v>88.72</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>79</v>
       </c>
@@ -1707,8 +2005,14 @@
       <c r="F36" s="10">
         <v>7.96</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>228</v>
+      </c>
+      <c r="H36" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>80</v>
       </c>
@@ -1724,8 +2028,14 @@
       <c r="F37" s="10">
         <v>7.66</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>228</v>
+      </c>
+      <c r="H37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>81</v>
       </c>
@@ -1741,8 +2051,14 @@
       <c r="F38" s="10">
         <v>468.6</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>228</v>
+      </c>
+      <c r="H38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>82</v>
       </c>
@@ -1758,8 +2074,15 @@
       <c r="F39" s="10">
         <v>126.5</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>228</v>
+      </c>
+      <c r="H39" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO39" s="17"/>
+    </row>
+    <row r="40" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
         <v>83</v>
       </c>
@@ -1775,8 +2098,15 @@
       <c r="F40" s="10">
         <v>12.38</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>224</v>
+      </c>
+      <c r="H40" t="s">
+        <v>200</v>
+      </c>
+      <c r="AO40" s="17"/>
+    </row>
+    <row r="41" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>84</v>
       </c>
@@ -1792,8 +2122,15 @@
       <c r="F41" s="10">
         <v>8.6300000000000008</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>224</v>
+      </c>
+      <c r="H41" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO41" s="17"/>
+    </row>
+    <row r="42" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>85</v>
       </c>
@@ -1809,8 +2146,15 @@
       <c r="F42" s="10">
         <v>89.35</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>224</v>
+      </c>
+      <c r="H42" t="s">
+        <v>202</v>
+      </c>
+      <c r="AO42" s="17"/>
+    </row>
+    <row r="43" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
         <v>86</v>
       </c>
@@ -1826,8 +2170,15 @@
       <c r="F43" s="10">
         <v>96.22</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>224</v>
+      </c>
+      <c r="H43" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO43" s="17"/>
+    </row>
+    <row r="44" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>101</v>
       </c>
@@ -1843,8 +2194,15 @@
       <c r="F44" s="10">
         <v>3.85</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>790</v>
+      </c>
+      <c r="H44" t="s">
+        <v>200</v>
+      </c>
+      <c r="AO44" s="17"/>
+    </row>
+    <row r="45" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>102</v>
       </c>
@@ -1860,8 +2218,15 @@
       <c r="F45" s="10">
         <v>10.14</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>790</v>
+      </c>
+      <c r="H45" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO45" s="17"/>
+    </row>
+    <row r="46" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>103</v>
       </c>
@@ -1877,8 +2242,15 @@
       <c r="F46" s="10">
         <v>379.7</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>790</v>
+      </c>
+      <c r="H46" t="s">
+        <v>202</v>
+      </c>
+      <c r="AO46" s="17"/>
+    </row>
+    <row r="47" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>104</v>
       </c>
@@ -1894,8 +2266,15 @@
       <c r="F47" s="10">
         <v>79.45</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>790</v>
+      </c>
+      <c r="H47" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO47" s="17"/>
+    </row>
+    <row r="48" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>105</v>
       </c>
@@ -1911,8 +2290,15 @@
       <c r="F48" s="11">
         <v>10.86</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>791</v>
+      </c>
+      <c r="H48" t="s">
+        <v>200</v>
+      </c>
+      <c r="AO48" s="17"/>
+    </row>
+    <row r="49" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>106</v>
       </c>
@@ -1928,8 +2314,15 @@
       <c r="F49" s="11">
         <v>19.55</v>
       </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>791</v>
+      </c>
+      <c r="H49" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO49" s="17"/>
+    </row>
+    <row r="50" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>107</v>
       </c>
@@ -1945,8 +2338,15 @@
       <c r="F50" s="11">
         <v>504</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>791</v>
+      </c>
+      <c r="H50" t="s">
+        <v>202</v>
+      </c>
+      <c r="AO50" s="17"/>
+    </row>
+    <row r="51" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>108</v>
       </c>
@@ -1962,8 +2362,15 @@
       <c r="F51" s="11">
         <v>103.9</v>
       </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>791</v>
+      </c>
+      <c r="H51" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO51" s="17"/>
+    </row>
+    <row r="52" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>109</v>
       </c>
@@ -1979,8 +2386,15 @@
       <c r="F52" s="11">
         <v>15.32</v>
       </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>792</v>
+      </c>
+      <c r="H52" t="s">
+        <v>200</v>
+      </c>
+      <c r="AO52" s="17"/>
+    </row>
+    <row r="53" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
         <v>110</v>
       </c>
@@ -1996,8 +2410,15 @@
       <c r="F53" s="11">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>792</v>
+      </c>
+      <c r="H53" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO53" s="17"/>
+    </row>
+    <row r="54" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>111</v>
       </c>
@@ -2013,8 +2434,15 @@
       <c r="F54" s="11">
         <v>191.2</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>792</v>
+      </c>
+      <c r="H54" t="s">
+        <v>202</v>
+      </c>
+      <c r="AO54" s="17"/>
+    </row>
+    <row r="55" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
         <v>112</v>
       </c>
@@ -2030,8 +2458,15 @@
       <c r="F55" s="11">
         <v>65.540000000000006</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>792</v>
+      </c>
+      <c r="H55" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO55" s="17"/>
+    </row>
+    <row r="56" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>113</v>
       </c>
@@ -2047,8 +2482,15 @@
       <c r="F56" s="11">
         <v>5.85</v>
       </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>793</v>
+      </c>
+      <c r="H56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AO56" s="17"/>
+    </row>
+    <row r="57" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
         <v>114</v>
       </c>
@@ -2064,8 +2506,15 @@
       <c r="F57" s="11">
         <v>5.55</v>
       </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>793</v>
+      </c>
+      <c r="H57" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO57" s="17"/>
+    </row>
+    <row r="58" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>115</v>
       </c>
@@ -2081,8 +2530,15 @@
       <c r="F58" s="11">
         <v>53.08</v>
       </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>793</v>
+      </c>
+      <c r="H58" t="s">
+        <v>202</v>
+      </c>
+      <c r="AO58" s="17"/>
+    </row>
+    <row r="59" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
         <v>116</v>
       </c>
@@ -2098,8 +2554,15 @@
       <c r="F59" s="11">
         <v>34.75</v>
       </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>793</v>
+      </c>
+      <c r="H59" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO59" s="17"/>
+    </row>
+    <row r="60" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
         <v>117</v>
       </c>
@@ -2115,8 +2578,18 @@
       <c r="F60" s="11">
         <v>331</v>
       </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60" t="s">
+        <v>204</v>
+      </c>
+      <c r="I60" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO60" s="17"/>
+    </row>
+    <row r="61" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
         <v>118</v>
       </c>
@@ -2132,8 +2605,18 @@
       <c r="F61" s="11">
         <v>160.5</v>
       </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61" t="s">
+        <v>204</v>
+      </c>
+      <c r="I61" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO61" s="17"/>
+    </row>
+    <row r="62" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B62" s="7" t="s">
         <v>151</v>
       </c>
@@ -2149,8 +2632,21 @@
       <c r="F62" s="11">
         <v>381.6</v>
       </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="H62" t="s">
+        <v>207</v>
+      </c>
+      <c r="I62" t="s">
+        <v>208</v>
+      </c>
+      <c r="J62" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO62" s="17"/>
+    </row>
+    <row r="63" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B63" s="7" t="s">
         <v>152</v>
       </c>
@@ -2166,8 +2662,21 @@
       <c r="F63" s="11">
         <v>484</v>
       </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>3</v>
+      </c>
+      <c r="H63" t="s">
+        <v>207</v>
+      </c>
+      <c r="I63" t="s">
+        <v>210</v>
+      </c>
+      <c r="J63" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO63" s="17"/>
+    </row>
+    <row r="64" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B64" s="7" t="s">
         <v>153</v>
       </c>
@@ -2183,8 +2692,21 @@
       <c r="F64" s="11">
         <v>363.6</v>
       </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>3</v>
+      </c>
+      <c r="H64" t="s">
+        <v>207</v>
+      </c>
+      <c r="I64" t="s">
+        <v>211</v>
+      </c>
+      <c r="J64" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO64" s="17"/>
+    </row>
+    <row r="65" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B65" s="7" t="s">
         <v>154</v>
       </c>
@@ -2200,8 +2722,21 @@
       <c r="F65" s="11">
         <v>130.69999999999999</v>
       </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="H65" t="s">
+        <v>207</v>
+      </c>
+      <c r="I65" t="s">
+        <v>212</v>
+      </c>
+      <c r="J65" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO65" s="17"/>
+    </row>
+    <row r="66" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B66" s="7" t="s">
         <v>155</v>
       </c>
@@ -2217,8 +2752,21 @@
       <c r="F66" s="11">
         <v>277.3</v>
       </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66" t="s">
+        <v>207</v>
+      </c>
+      <c r="I66" t="s">
+        <v>213</v>
+      </c>
+      <c r="J66" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO66" s="17"/>
+    </row>
+    <row r="67" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B67" s="7" t="s">
         <v>156</v>
       </c>
@@ -2234,8 +2782,21 @@
       <c r="F67" s="11">
         <v>222</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67" t="s">
+        <v>207</v>
+      </c>
+      <c r="I67" t="s">
+        <v>214</v>
+      </c>
+      <c r="J67" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO67" s="17"/>
+    </row>
+    <row r="68" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B68" s="7" t="s">
         <v>157</v>
       </c>
@@ -2251,8 +2812,21 @@
       <c r="F68" s="11">
         <v>100</v>
       </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68" t="s">
+        <v>207</v>
+      </c>
+      <c r="I68" t="s">
+        <v>215</v>
+      </c>
+      <c r="J68" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO68" s="17"/>
+    </row>
+    <row r="69" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B69" s="7" t="s">
         <v>158</v>
       </c>
@@ -2268,8 +2842,21 @@
       <c r="F69" s="11">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="H69" t="s">
+        <v>207</v>
+      </c>
+      <c r="I69" t="s">
+        <v>216</v>
+      </c>
+      <c r="J69" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO69" s="17"/>
+    </row>
+    <row r="70" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B70" s="7" t="s">
         <v>159</v>
       </c>
@@ -2285,8 +2872,21 @@
       <c r="F70" s="11">
         <v>75.28</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70" t="s">
+        <v>207</v>
+      </c>
+      <c r="I70" t="s">
+        <v>217</v>
+      </c>
+      <c r="J70" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO70" s="17"/>
+    </row>
+    <row r="71" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B71" s="7" t="s">
         <v>160</v>
       </c>
@@ -2302,8 +2902,21 @@
       <c r="F71" s="11">
         <v>71.05</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>3</v>
+      </c>
+      <c r="H71" t="s">
+        <v>207</v>
+      </c>
+      <c r="I71" t="s">
+        <v>218</v>
+      </c>
+      <c r="J71" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO71" s="17"/>
+    </row>
+    <row r="72" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B72" s="8" t="s">
         <v>161</v>
       </c>
@@ -2319,8 +2932,21 @@
       <c r="F72" s="11">
         <v>614.9</v>
       </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>7</v>
+      </c>
+      <c r="H72" t="s">
+        <v>207</v>
+      </c>
+      <c r="I72" t="s">
+        <v>208</v>
+      </c>
+      <c r="J72" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO72" s="17"/>
+    </row>
+    <row r="73" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B73" s="8" t="s">
         <v>162</v>
       </c>
@@ -2336,8 +2962,21 @@
       <c r="F73" s="11">
         <v>726</v>
       </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>7</v>
+      </c>
+      <c r="H73" t="s">
+        <v>207</v>
+      </c>
+      <c r="I73" t="s">
+        <v>210</v>
+      </c>
+      <c r="J73" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO73" s="17"/>
+    </row>
+    <row r="74" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B74" s="8" t="s">
         <v>163</v>
       </c>
@@ -2353,8 +2992,21 @@
       <c r="F74" s="11">
         <v>329</v>
       </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>7</v>
+      </c>
+      <c r="H74" t="s">
+        <v>207</v>
+      </c>
+      <c r="I74" t="s">
+        <v>211</v>
+      </c>
+      <c r="J74" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO74" s="17"/>
+    </row>
+    <row r="75" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B75" s="8" t="s">
         <v>164</v>
       </c>
@@ -2370,8 +3022,21 @@
       <c r="F75" s="11">
         <v>414</v>
       </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>7</v>
+      </c>
+      <c r="H75" t="s">
+        <v>207</v>
+      </c>
+      <c r="I75" t="s">
+        <v>212</v>
+      </c>
+      <c r="J75" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO75" s="17"/>
+    </row>
+    <row r="76" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B76" s="8" t="s">
         <v>165</v>
       </c>
@@ -2387,8 +3052,20 @@
       <c r="F76" s="11">
         <v>414.1</v>
       </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>7</v>
+      </c>
+      <c r="H76" t="s">
+        <v>207</v>
+      </c>
+      <c r="I76" t="s">
+        <v>213</v>
+      </c>
+      <c r="J76" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B77" s="8" t="s">
         <v>166</v>
       </c>
@@ -2404,8 +3081,20 @@
       <c r="F77" s="11">
         <v>30.06</v>
       </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>7</v>
+      </c>
+      <c r="H77" t="s">
+        <v>207</v>
+      </c>
+      <c r="I77" t="s">
+        <v>214</v>
+      </c>
+      <c r="J77" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="78" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B78" s="8" t="s">
         <v>167</v>
       </c>
@@ -2421,8 +3110,20 @@
       <c r="F78" s="11">
         <v>57.4</v>
       </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G78">
+        <v>7</v>
+      </c>
+      <c r="H78" t="s">
+        <v>207</v>
+      </c>
+      <c r="I78" t="s">
+        <v>215</v>
+      </c>
+      <c r="J78" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="79" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B79" s="8" t="s">
         <v>168</v>
       </c>
@@ -2438,8 +3139,20 @@
       <c r="F79" s="11">
         <v>101.9</v>
       </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G79">
+        <v>7</v>
+      </c>
+      <c r="H79" t="s">
+        <v>207</v>
+      </c>
+      <c r="I79" t="s">
+        <v>216</v>
+      </c>
+      <c r="J79" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="80" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B80" s="8" t="s">
         <v>169</v>
       </c>
@@ -2455,8 +3168,20 @@
       <c r="F80" s="11">
         <v>25.96</v>
       </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <v>7</v>
+      </c>
+      <c r="H80" t="s">
+        <v>207</v>
+      </c>
+      <c r="I80" t="s">
+        <v>217</v>
+      </c>
+      <c r="J80" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B81" s="8" t="s">
         <v>170</v>
       </c>
@@ -2472,8 +3197,20 @@
       <c r="F81" s="11">
         <v>158.69999999999999</v>
       </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G81">
+        <v>7</v>
+      </c>
+      <c r="H81" t="s">
+        <v>207</v>
+      </c>
+      <c r="I81" t="s">
+        <v>218</v>
+      </c>
+      <c r="J81" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B82" s="9" t="s">
         <v>171</v>
       </c>
@@ -2489,8 +3226,20 @@
       <c r="F82" s="11">
         <v>826</v>
       </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <v>14</v>
+      </c>
+      <c r="H82" t="s">
+        <v>207</v>
+      </c>
+      <c r="I82" t="s">
+        <v>208</v>
+      </c>
+      <c r="J82" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B83" s="9" t="s">
         <v>172</v>
       </c>
@@ -2506,8 +3255,20 @@
       <c r="F83" s="11">
         <v>313.89999999999998</v>
       </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G83">
+        <v>14</v>
+      </c>
+      <c r="H83" t="s">
+        <v>207</v>
+      </c>
+      <c r="I83" t="s">
+        <v>210</v>
+      </c>
+      <c r="J83" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B84" s="9" t="s">
         <v>173</v>
       </c>
@@ -2523,8 +3284,20 @@
       <c r="F84" s="11">
         <v>518</v>
       </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G84">
+        <v>14</v>
+      </c>
+      <c r="H84" t="s">
+        <v>207</v>
+      </c>
+      <c r="I84" t="s">
+        <v>211</v>
+      </c>
+      <c r="J84" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B85" s="9" t="s">
         <v>174</v>
       </c>
@@ -2540,8 +3313,20 @@
       <c r="F85" s="11">
         <v>350</v>
       </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G85">
+        <v>14</v>
+      </c>
+      <c r="H85" t="s">
+        <v>207</v>
+      </c>
+      <c r="I85" t="s">
+        <v>212</v>
+      </c>
+      <c r="J85" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B86" s="9" t="s">
         <v>175</v>
       </c>
@@ -2557,8 +3342,20 @@
       <c r="F86" s="11">
         <v>116.9</v>
       </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G86">
+        <v>14</v>
+      </c>
+      <c r="H86" t="s">
+        <v>207</v>
+      </c>
+      <c r="I86" t="s">
+        <v>213</v>
+      </c>
+      <c r="J86" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B87" s="9" t="s">
         <v>176</v>
       </c>
@@ -2574,8 +3371,20 @@
       <c r="F87" s="11">
         <v>58.94</v>
       </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G87">
+        <v>14</v>
+      </c>
+      <c r="H87" t="s">
+        <v>207</v>
+      </c>
+      <c r="I87" t="s">
+        <v>214</v>
+      </c>
+      <c r="J87" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B88" s="9" t="s">
         <v>177</v>
       </c>
@@ -2591,8 +3400,20 @@
       <c r="F88" s="11">
         <v>22.27</v>
       </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G88">
+        <v>14</v>
+      </c>
+      <c r="H88" t="s">
+        <v>207</v>
+      </c>
+      <c r="I88" t="s">
+        <v>215</v>
+      </c>
+      <c r="J88" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B89" s="9" t="s">
         <v>178</v>
       </c>
@@ -2608,8 +3429,20 @@
       <c r="F89" s="11">
         <v>20.32</v>
       </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G89">
+        <v>14</v>
+      </c>
+      <c r="H89" t="s">
+        <v>207</v>
+      </c>
+      <c r="I89" t="s">
+        <v>216</v>
+      </c>
+      <c r="J89" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B90" s="9" t="s">
         <v>179</v>
       </c>
@@ -2625,8 +3458,20 @@
       <c r="F90" s="11">
         <v>87.24</v>
       </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G90">
+        <v>14</v>
+      </c>
+      <c r="H90" t="s">
+        <v>207</v>
+      </c>
+      <c r="I90" t="s">
+        <v>217</v>
+      </c>
+      <c r="J90" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B91" s="9" t="s">
         <v>180</v>
       </c>
@@ -2641,6 +3486,18 @@
       </c>
       <c r="F91" s="11">
         <v>153.30000000000001</v>
+      </c>
+      <c r="G91">
+        <v>14</v>
+      </c>
+      <c r="H91" t="s">
+        <v>207</v>
+      </c>
+      <c r="I91" t="s">
+        <v>218</v>
+      </c>
+      <c r="J91" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>